<commit_message>
made some small changes and removed extra things from the excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestNG_data.xlsx
+++ b/src/test/resources/testData/TestNG_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDE69B9-DE7D-AF4D-8C86-3C645B1797F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B142D9-FACE-5243-BA89-A39D9619233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1320" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1480" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -205,22 +205,14 @@
 print(sortedSquares([-7, -3, 2, 3, 11]))</t>
   </si>
   <si>
-    <t>def findNumbers(nums):
-  count = 0
-  for num in nums:
-    if len(str(num)) % 2 == 0:
-      count += 1
-      return count
-numsArr1 = [12, 345, 2, 6, 7896]
-print("Even number of digits in given array")
-print (findNumbers(numsArr1))</t>
+    <t>Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,12 +244,6 @@
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -285,12 +271,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -347,9 +327,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -360,7 +340,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -372,29 +352,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -678,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -692,12 +668,11 @@
     <col min="4" max="4" width="30.83203125" customWidth="1"/>
     <col min="5" max="5" width="44.1640625" customWidth="1"/>
     <col min="6" max="6" width="43" customWidth="1"/>
-    <col min="7" max="7" width="36.1640625" customWidth="1"/>
-    <col min="8" max="8" width="26.5" customWidth="1"/>
-    <col min="9" max="9" width="40.5" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
+    <col min="8" max="8" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16" thickBot="1">
+    <row r="1" spans="1:8" ht="16" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,16 +692,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18" thickBot="1">
+    <row r="2" spans="1:8" ht="17" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -742,12 +714,11 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" thickBot="1">
+    <row r="3" spans="1:8" ht="17" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -755,16 +726,15 @@
         <v>12</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" ht="17" thickBot="1">
+    </row>
+    <row r="4" spans="1:8" ht="17" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -781,9 +751,8 @@
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" ht="17" thickBot="1">
+    </row>
+    <row r="5" spans="1:8" ht="17" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
@@ -798,102 +767,88 @@
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="151" thickBot="1">
-      <c r="A6" s="9" t="s">
-        <v>43</v>
+    </row>
+    <row r="6" spans="1:8" ht="17" thickBot="1">
+      <c r="A6" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>17</v>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" ht="241" thickBot="1">
-      <c r="A7" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="17" thickBot="1">
+      <c r="A7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>17</v>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" ht="136" thickBot="1">
-      <c r="A8" s="9" t="s">
-        <v>47</v>
+    </row>
+    <row r="8" spans="1:8" ht="17" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>17</v>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="76" thickBot="1">
-      <c r="A9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="17" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>17</v>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1">
-      <c r="A10" s="9" t="s">
-        <v>21</v>
+    </row>
+    <row r="10" spans="1:8" ht="17" thickBot="1">
+      <c r="A10" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" ht="17" thickBot="1">
-      <c r="A11" s="9" t="s">
-        <v>23</v>
+      <c r="G10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="17" thickBot="1">
+      <c r="A11" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>24</v>
@@ -902,148 +857,76 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="17" thickBot="1">
-      <c r="A12" s="9" t="s">
-        <v>25</v>
+      <c r="G11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="17" thickBot="1">
+      <c r="A12" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" ht="17" thickBot="1">
-      <c r="A13" s="9" t="s">
-        <v>27</v>
+      <c r="G12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1">
+      <c r="A13" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1">
-      <c r="A14" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="G13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="17" thickBot="1">
+      <c r="A14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" ht="17" thickBot="1">
-      <c r="A15" s="9" t="s">
-        <v>30</v>
+      <c r="G14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" thickBot="1">
+      <c r="A15" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" ht="17" thickBot="1">
-      <c r="A16" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" ht="17" thickBot="1">
-      <c r="A17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" ht="18" thickBot="1">
-      <c r="A18" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="16">
-      <c r="A19" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="15" t="s">
+      <c r="H15" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1059,10 +942,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7230CE01-58C0-5943-8B86-17F9BFE5E4D6}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1076,85 +959,87 @@
     <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31" thickBot="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" ht="31" thickBot="1">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="282" customHeight="1" thickBot="1">
-      <c r="A2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="16" t="s">
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" ht="282" customHeight="1" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" thickBot="1">
-      <c r="A3" s="9" t="s">
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" ht="16" thickBot="1">
+      <c r="A3" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" customHeight="1" thickBot="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:7" ht="90" customHeight="1" thickBot="1">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" thickBot="1">
+    <row r="5" spans="1:7" ht="16" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing practice q code for array
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestNG_data.xlsx
+++ b/src/test/resources/testData/TestNG_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B142D9-FACE-5243-BA89-A39D9619233F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE70F462-D57E-C749-A00E-04C4E50F67F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1480" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="4300" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -76,16 +76,6 @@
   </si>
   <si>
     <t>Submission Successful</t>
-  </si>
-  <si>
-    <t>The maximum number of consecutive 1's in input1 is: 
-2
-The maximum number of consecutive 1's in input2 is: 
-1</t>
-  </si>
-  <si>
-    <t>Even number of digits in given array
-1</t>
   </si>
   <si>
     <t>[0, 1, 9, 16, 100]
@@ -174,24 +164,6 @@
 print(search([12, 23, 45, 67, 6, 90], 25))   # Output: Not Found</t>
   </si>
   <si>
-    <t>def findMaxConsecutiveOnes(nums) :
-  maxCount=0
-  currentCount=0
-  for n in nums:
-    if(n==1):
-      currentCount+=1
-      maxCount=max(maxCount,currentCount)
-    else:
-      currentCount=0
-      return maxCount
-input1=[1,1,0,1,1,1]
-input2=[1,0,1,1,0,1]
-print("The maximum number of consecutive 1's in input1 is: ")
-print(findMaxConsecutiveOnes(input1))
-print("The maximum number of consecutive 1's in input2 is: ")
-print(findMaxConsecutiveOnes(input2))</t>
-  </si>
-  <si>
     <t>PracticeQ3validcode</t>
   </si>
   <si>
@@ -207,12 +179,49 @@
   <si>
     <t>Code</t>
   </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    max_count = 0
+    current_count = 0
+    for num in nums:
+        if num == 1:
+            current_count += 1
+            max_count = max(max_count, current_count)
+        else:
+            current_count = 0  # reset when 0 is found
+    return max_count
+# Example usage:
+print(findMaxConsecutiveOnes([1,1,0,1,1,1]))  # Output: 3
+print(findMaxConsecutiveOnes([1,0,1,1,0,1]))  # Output: 2</t>
+  </si>
+  <si>
+    <t>3
+2</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+    count = 0
+    for num in nums:
+        if len(str(num)) % 2 == 0:
+            count += 1
+    return count
+# Example usage:
+print(findNumbers([12, 345, 2, 6, 7896]))   # Output: 2
+print(findNumbers([555, 901, 482, 1771]))  # Output: 1</t>
+  </si>
+  <si>
+    <t>2
+1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,11 +262,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Play"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arimo"/>
     </font>
     <font>
       <sz val="10"/>
@@ -327,9 +331,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -340,7 +344,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -365,12 +369,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -700,7 +701,7 @@
     </row>
     <row r="2" spans="1:8" ht="17" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -720,7 +721,7 @@
     </row>
     <row r="3" spans="1:8" ht="17" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
@@ -736,7 +737,7 @@
     </row>
     <row r="4" spans="1:8" ht="17" thickBot="1">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -754,7 +755,7 @@
     </row>
     <row r="5" spans="1:8" ht="17" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -763,14 +764,14 @@
         <v>14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="17" thickBot="1">
       <c r="A6" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -778,93 +779,93 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="17" thickBot="1">
       <c r="A7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="17" thickBot="1">
       <c r="A8" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="17" thickBot="1">
       <c r="A9" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" ht="17" thickBot="1">
       <c r="A10" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="13" t="s">
-        <v>41</v>
+      <c r="G10" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1">
       <c r="A11" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="13" t="s">
-        <v>41</v>
+      <c r="G11" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="17" thickBot="1">
       <c r="A12" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="5" t="s">
@@ -873,17 +874,17 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="13" t="s">
-        <v>41</v>
+      <c r="G12" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" ht="17" thickBot="1">
       <c r="A13" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>10</v>
@@ -891,17 +892,17 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="13" t="s">
-        <v>41</v>
+      <c r="G13" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="17" thickBot="1">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>10</v>
@@ -909,16 +910,16 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>35</v>
+      <c r="G14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16" thickBot="1">
       <c r="A15" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>9</v>
@@ -926,7 +927,7 @@
       <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -945,7 +946,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -964,37 +965,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="282" customHeight="1" thickBot="1">
       <c r="A2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>14</v>
@@ -1003,7 +1006,7 @@
     </row>
     <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>14</v>
@@ -1011,19 +1014,25 @@
     </row>
     <row r="4" spans="1:7" ht="90" customHeight="1" thickBot="1">
       <c r="A4" s="8" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>20</v>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" thickBot="1">

</xml_diff>

<commit_message>
made some naming changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestNG_data.xlsx
+++ b/src/test/resources/testData/TestNG_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE70F462-D57E-C749-A00E-04C4E50F67F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F6E0C0-A0BB-4A48-9710-EA21099D8859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="4300" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="2100" windowWidth="27720" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -943,10 +943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7230CE01-58C0-5943-8B86-17F9BFE5E4D6}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1035,23 +1035,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16" thickBot="1">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>